<commit_message>
Atualização automática de ALVORADA.xlsx
</commit_message>
<xml_diff>
--- a/ALVORADA.xlsx
+++ b/ALVORADA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{140E4225-45BE-4E87-91B0-5C72EFA032C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E060703-7696-40F2-A909-DA74C192E6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1578,7 +1565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1638,36 +1625,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1706,14 +1669,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1767,7 +1725,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{68F3ABAD-5C48-43E1-98E8-5A61375201D6}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{9D6AB2B8-B6D6-4C59-977F-CC19FE3CF167}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1797,10 +1755,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E184AB5D-3752-4FFA-B541-4EAAF1B8E3FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51602F98-F23C-40D4-9E07-0B5B8B2C1235}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1838,7 +1796,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15995711-07E9-4AB7-9496-6BD47C3B46C8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6694E89E-B686-42C4-B3C1-85FF9B73D50F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1901,7 +1859,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBBBCC22-797D-4028-8BD5-C803CB6D5C3B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A371CF89-ECCC-4659-AD57-70261ECF46D2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1920,7 +1878,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76CAF859-919D-1989-5F59-227A7C72A657}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DF32B0A-AB2E-4888-6F85-0F358443BC86}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1969,7 +1927,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18C0D49-0EB3-6638-4178-5F3B0B4EDF24}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0E0C4CF-CD49-64BF-4836-BB4D9F404F51}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1988,7 +1946,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2B8EC27-4433-9724-2EAA-9B1D8EB007BA}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6BEB948-F291-13B6-F306-643DE80D1D1B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2019,7 +1977,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FEEAC6D-7681-0269-4F42-0901233B8FFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7585004E-CE41-DF3F-7BB8-398D5E25C135}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2050,7 +2008,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8175A6A2-25A7-BCD2-C3EE-145F637A7C07}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090DA6D7-E731-E808-CEE3-9D286D3C73ED}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2093,7 +2051,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F75ECF0-7A39-434A-A9F2-06630C442CA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B63E4719-9C6C-47BC-BBA8-5997F4C80D4D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2131,7 +2089,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322799E2-23D2-41E5-B8EE-8325CCCEA8EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7EB3A06-F026-4341-929F-500AAF780D95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2174,7 +2132,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{369B37D1-ECE6-46D6-AE28-975DA4CBC817}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DB2E190-4E09-4D1E-A422-4DFBCDB70781}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2487,7 +2445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59FA0262-98F7-4006-BC26-79CE897BC952}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D724ADDD-2068-49BB-A6B3-0084C9E02E2F}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2499,98 +2457,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5856,19 +5814,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5891,46 +5849,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>280</v>
       </c>
     </row>
@@ -5948,16 +5906,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5991,7 +5949,7 @@
       <c r="J1" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="21" t="s">
         <v>291</v>
       </c>
     </row>
@@ -6005,10 +5963,10 @@
       <c r="C2" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>190</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>19</v>
       </c>
       <c r="F2" s="2">
@@ -6026,7 +5984,7 @@
       <c r="J2" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -6040,10 +5998,10 @@
       <c r="C3" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>32</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>3.2</v>
       </c>
       <c r="F3" s="2">
@@ -6061,7 +6019,7 @@
       <c r="J3" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -6075,10 +6033,10 @@
       <c r="C4" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>154.16</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>15.42</v>
       </c>
       <c r="F4" s="2">
@@ -6096,7 +6054,7 @@
       <c r="J4" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -6110,10 +6068,10 @@
       <c r="C5" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="22">
         <v>154.02000000000001</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <v>15.4</v>
       </c>
       <c r="F5" s="2">
@@ -6131,7 +6089,7 @@
       <c r="J5" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="23">
         <v>9612</v>
       </c>
     </row>
@@ -6145,10 +6103,10 @@
       <c r="C6" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>154.02000000000001</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>15.4</v>
       </c>
       <c r="F6" s="2">
@@ -6166,7 +6124,7 @@
       <c r="J6" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -6180,10 +6138,10 @@
       <c r="C7" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>154.02000000000001</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>15.4</v>
       </c>
       <c r="F7" s="2">
@@ -6201,7 +6159,7 @@
       <c r="J7" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="23">
         <v>9612</v>
       </c>
     </row>
@@ -6215,10 +6173,10 @@
       <c r="C8" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>154.02000000000001</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>0</v>
       </c>
       <c r="F8" s="2">
@@ -6236,7 +6194,7 @@
       <c r="J8" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="23">
         <v>11465</v>
       </c>
     </row>
@@ -6250,10 +6208,10 @@
       <c r="C9" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <v>154.02000000000001</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>15.4</v>
       </c>
       <c r="F9" s="2">
@@ -6271,7 +6229,7 @@
       <c r="J9" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="23">
         <v>9612</v>
       </c>
     </row>
@@ -6285,10 +6243,10 @@
       <c r="C10" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>136.5</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>13.65</v>
       </c>
       <c r="F10" s="2">
@@ -6306,7 +6264,7 @@
       <c r="J10" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="23">
         <v>19422</v>
       </c>
     </row>
@@ -6320,10 +6278,10 @@
       <c r="C11" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>93</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="22">
         <v>9.3000000000000007</v>
       </c>
       <c r="F11" s="2">
@@ -6341,7 +6299,7 @@
       <c r="J11" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="23">
         <v>12441</v>
       </c>
     </row>
@@ -6355,10 +6313,10 @@
       <c r="C12" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>125.4</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>12.54</v>
       </c>
       <c r="F12" s="2">
@@ -6376,7 +6334,7 @@
       <c r="J12" s="2" t="s">
         <v>315</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="23">
         <v>17276</v>
       </c>
     </row>
@@ -6390,10 +6348,10 @@
       <c r="C13" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <v>111</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>11.1</v>
       </c>
       <c r="F13" s="2">
@@ -6411,7 +6369,7 @@
       <c r="J13" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="23">
         <v>504</v>
       </c>
     </row>
@@ -6425,10 +6383,10 @@
       <c r="C14" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>2252.35</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>225.24</v>
       </c>
       <c r="F14" s="2">
@@ -6446,7 +6404,7 @@
       <c r="J14" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="23">
         <v>506</v>
       </c>
     </row>
@@ -6460,10 +6418,10 @@
       <c r="C15" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <v>136.65</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>13.67</v>
       </c>
       <c r="F15" s="2">
@@ -6481,7 +6439,7 @@
       <c r="J15" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="23">
         <v>6</v>
       </c>
     </row>
@@ -6495,10 +6453,10 @@
       <c r="C16" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>475.02</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>47.5</v>
       </c>
       <c r="F16" s="2">
@@ -6516,7 +6474,7 @@
       <c r="J16" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -6530,10 +6488,10 @@
       <c r="C17" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>493</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>49.3</v>
       </c>
       <c r="F17" s="2">
@@ -6551,7 +6509,7 @@
       <c r="J17" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="23">
         <v>26893</v>
       </c>
     </row>
@@ -6565,10 +6523,10 @@
       <c r="C18" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>390</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>39</v>
       </c>
       <c r="F18" s="2">
@@ -6586,7 +6544,7 @@
       <c r="J18" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="23">
         <v>26893</v>
       </c>
     </row>
@@ -6600,10 +6558,10 @@
       <c r="C19" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <v>480.1</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>48.01</v>
       </c>
       <c r="F19" s="2">
@@ -6621,7 +6579,7 @@
       <c r="J19" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -6635,10 +6593,10 @@
       <c r="C20" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>185</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>18.5</v>
       </c>
       <c r="F20" s="2">
@@ -6656,7 +6614,7 @@
       <c r="J20" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -6670,10 +6628,10 @@
       <c r="C21" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>234</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="22">
         <v>23.4</v>
       </c>
       <c r="F21" s="2">
@@ -6691,7 +6649,7 @@
       <c r="J21" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="K21" s="26">
+      <c r="K21" s="23">
         <v>17478</v>
       </c>
     </row>
@@ -6705,10 +6663,10 @@
       <c r="C22" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>130</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>13</v>
       </c>
       <c r="F22" s="2">
@@ -6726,7 +6684,7 @@
       <c r="J22" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="23">
         <v>1373</v>
       </c>
     </row>
@@ -6740,10 +6698,10 @@
       <c r="C23" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>450</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>45</v>
       </c>
       <c r="F23" s="2">
@@ -6761,7 +6719,7 @@
       <c r="J23" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K23" s="26">
+      <c r="K23" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -6775,10 +6733,10 @@
       <c r="C24" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>350</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>35</v>
       </c>
       <c r="F24" s="2">
@@ -6796,7 +6754,7 @@
       <c r="J24" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K24" s="26">
+      <c r="K24" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -6810,10 +6768,10 @@
       <c r="C25" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>562.07000000000005</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="22">
         <v>56.21</v>
       </c>
       <c r="F25" s="2">
@@ -6831,7 +6789,7 @@
       <c r="J25" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K25" s="26">
+      <c r="K25" s="23">
         <v>505</v>
       </c>
     </row>
@@ -6845,10 +6803,10 @@
       <c r="C26" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <v>131.80000000000001</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <v>13.18</v>
       </c>
       <c r="F26" s="2">
@@ -6866,7 +6824,7 @@
       <c r="J26" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K26" s="26">
+      <c r="K26" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -6880,10 +6838,10 @@
       <c r="C27" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <v>902</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <v>180.4</v>
       </c>
       <c r="F27" s="2">
@@ -6901,7 +6859,7 @@
       <c r="J27" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K27" s="26">
+      <c r="K27" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -6915,10 +6873,10 @@
       <c r="C28" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>367</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <v>36.700000000000003</v>
       </c>
       <c r="F28" s="2">
@@ -6936,7 +6894,7 @@
       <c r="J28" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="23">
         <v>17478</v>
       </c>
     </row>
@@ -6950,10 +6908,10 @@
       <c r="C29" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <v>300</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="22">
         <v>30</v>
       </c>
       <c r="F29" s="2">
@@ -6971,7 +6929,7 @@
       <c r="J29" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="23">
         <v>504</v>
       </c>
     </row>
@@ -6985,10 +6943,10 @@
       <c r="C30" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>593.27</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>353.51</v>
       </c>
       <c r="F30" s="2">
@@ -7006,7 +6964,7 @@
       <c r="J30" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K30" s="26">
+      <c r="K30" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -7020,10 +6978,10 @@
       <c r="C31" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <v>600</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="22">
         <v>60</v>
       </c>
       <c r="F31" s="2">
@@ -7041,7 +6999,7 @@
       <c r="J31" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="23">
         <v>11465</v>
       </c>
     </row>
@@ -7055,10 +7013,10 @@
       <c r="C32" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="22">
         <v>600</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="22">
         <v>0</v>
       </c>
       <c r="F32" s="2">
@@ -7076,7 +7034,7 @@
       <c r="J32" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="K32" s="26">
+      <c r="K32" s="23">
         <v>10249</v>
       </c>
     </row>
@@ -7090,10 +7048,10 @@
       <c r="C33" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="22">
         <v>190</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="22">
         <v>19</v>
       </c>
       <c r="F33" s="2">
@@ -7111,7 +7069,7 @@
       <c r="J33" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K33" s="26">
+      <c r="K33" s="23">
         <v>11448</v>
       </c>
     </row>
@@ -7125,10 +7083,10 @@
       <c r="C34" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="22">
         <v>80</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="22">
         <v>8</v>
       </c>
       <c r="F34" s="2">
@@ -7146,7 +7104,7 @@
       <c r="J34" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K34" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7160,10 +7118,10 @@
       <c r="C35" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="22">
         <v>96.8</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="22">
         <v>9.68</v>
       </c>
       <c r="F35" s="2">
@@ -7181,7 +7139,7 @@
       <c r="J35" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K35" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7195,10 +7153,10 @@
       <c r="C36" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="D36" s="25">
+      <c r="D36" s="22">
         <v>96.8</v>
       </c>
-      <c r="E36" s="25">
+      <c r="E36" s="22">
         <v>9.68</v>
       </c>
       <c r="F36" s="2">
@@ -7216,7 +7174,7 @@
       <c r="J36" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="K36" s="26">
+      <c r="K36" s="23">
         <v>13987</v>
       </c>
     </row>
@@ -7230,10 +7188,10 @@
       <c r="C37" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D37" s="25">
+      <c r="D37" s="22">
         <v>81.66</v>
       </c>
-      <c r="E37" s="25">
+      <c r="E37" s="22">
         <v>8.17</v>
       </c>
       <c r="F37" s="2">
@@ -7251,7 +7209,7 @@
       <c r="J37" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K37" s="26">
+      <c r="K37" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7265,10 +7223,10 @@
       <c r="C38" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D38" s="25">
+      <c r="D38" s="22">
         <v>81.66</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="22">
         <v>8.17</v>
       </c>
       <c r="F38" s="2">
@@ -7286,7 +7244,7 @@
       <c r="J38" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K38" s="26">
+      <c r="K38" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7300,10 +7258,10 @@
       <c r="C39" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D39" s="25">
+      <c r="D39" s="22">
         <v>81.66</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="22">
         <v>8.17</v>
       </c>
       <c r="F39" s="2">
@@ -7321,7 +7279,7 @@
       <c r="J39" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K39" s="26">
+      <c r="K39" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7335,10 +7293,10 @@
       <c r="C40" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D40" s="25">
+      <c r="D40" s="22">
         <v>81.66</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="22">
         <v>8.17</v>
       </c>
       <c r="F40" s="2">
@@ -7356,7 +7314,7 @@
       <c r="J40" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K40" s="26">
+      <c r="K40" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7370,10 +7328,10 @@
       <c r="C41" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="22">
         <v>81.66</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="22">
         <v>8.17</v>
       </c>
       <c r="F41" s="2">
@@ -7391,7 +7349,7 @@
       <c r="J41" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K41" s="26">
+      <c r="K41" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7405,10 +7363,10 @@
       <c r="C42" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D42" s="25">
+      <c r="D42" s="22">
         <v>62</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="22">
         <v>6.2</v>
       </c>
       <c r="F42" s="2">
@@ -7426,7 +7384,7 @@
       <c r="J42" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K42" s="26">
+      <c r="K42" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7440,10 +7398,10 @@
       <c r="C43" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D43" s="25">
+      <c r="D43" s="22">
         <v>62</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="22">
         <v>6.2</v>
       </c>
       <c r="F43" s="2">
@@ -7461,7 +7419,7 @@
       <c r="J43" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K43" s="26">
+      <c r="K43" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7475,10 +7433,10 @@
       <c r="C44" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="D44" s="25">
+      <c r="D44" s="22">
         <v>62</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="22">
         <v>6.2</v>
       </c>
       <c r="F44" s="2">
@@ -7496,7 +7454,7 @@
       <c r="J44" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7510,10 +7468,10 @@
       <c r="C45" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D45" s="25">
+      <c r="D45" s="22">
         <v>59</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="22">
         <v>5.9</v>
       </c>
       <c r="F45" s="2">
@@ -7531,7 +7489,7 @@
       <c r="J45" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K45" s="26">
+      <c r="K45" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -7545,10 +7503,10 @@
       <c r="C46" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D46" s="25">
+      <c r="D46" s="22">
         <v>59</v>
       </c>
-      <c r="E46" s="25">
+      <c r="E46" s="22">
         <v>5.9</v>
       </c>
       <c r="F46" s="2">
@@ -7566,7 +7524,7 @@
       <c r="J46" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K46" s="26">
+      <c r="K46" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7580,10 +7538,10 @@
       <c r="C47" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D47" s="25">
+      <c r="D47" s="22">
         <v>59</v>
       </c>
-      <c r="E47" s="25">
+      <c r="E47" s="22">
         <v>0</v>
       </c>
       <c r="F47" s="2">
@@ -7601,7 +7559,7 @@
       <c r="J47" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K47" s="26">
+      <c r="K47" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7615,10 +7573,10 @@
       <c r="C48" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D48" s="25">
+      <c r="D48" s="22">
         <v>59</v>
       </c>
-      <c r="E48" s="25">
+      <c r="E48" s="22">
         <v>5.9</v>
       </c>
       <c r="F48" s="2">
@@ -7636,7 +7594,7 @@
       <c r="J48" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K48" s="26">
+      <c r="K48" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7650,10 +7608,10 @@
       <c r="C49" s="2" t="s">
         <v>355</v>
       </c>
-      <c r="D49" s="25">
+      <c r="D49" s="22">
         <v>59</v>
       </c>
-      <c r="E49" s="25">
+      <c r="E49" s="22">
         <v>5.9</v>
       </c>
       <c r="F49" s="2">
@@ -7671,7 +7629,7 @@
       <c r="J49" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K49" s="26">
+      <c r="K49" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -7685,10 +7643,10 @@
       <c r="C50" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="D50" s="25">
+      <c r="D50" s="22">
         <v>77.8</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="22">
         <v>7.78</v>
       </c>
       <c r="F50" s="2">
@@ -7706,7 +7664,7 @@
       <c r="J50" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K50" s="26">
+      <c r="K50" s="23">
         <v>13744</v>
       </c>
     </row>
@@ -7720,10 +7678,10 @@
       <c r="C51" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="D51" s="25">
+      <c r="D51" s="22">
         <v>77.8</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="22">
         <v>0</v>
       </c>
       <c r="F51" s="2">
@@ -7741,7 +7699,7 @@
       <c r="J51" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K51" s="26">
+      <c r="K51" s="23">
         <v>13744</v>
       </c>
     </row>
@@ -7755,10 +7713,10 @@
       <c r="C52" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D52" s="22">
         <v>36</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="22">
         <v>3.6</v>
       </c>
       <c r="F52" s="2">
@@ -7776,7 +7734,7 @@
       <c r="J52" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K52" s="26">
+      <c r="K52" s="23">
         <v>11448</v>
       </c>
     </row>
@@ -7790,10 +7748,10 @@
       <c r="C53" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D53" s="25">
+      <c r="D53" s="22">
         <v>32</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="22">
         <v>3.2</v>
       </c>
       <c r="F53" s="2">
@@ -7811,7 +7769,7 @@
       <c r="J53" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K53" s="26">
+      <c r="K53" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -7825,10 +7783,10 @@
       <c r="C54" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D54" s="25">
+      <c r="D54" s="22">
         <v>32</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="22">
         <v>3.2</v>
       </c>
       <c r="F54" s="2">
@@ -7846,7 +7804,7 @@
       <c r="J54" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K54" s="26">
+      <c r="K54" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -7860,10 +7818,10 @@
       <c r="C55" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D55" s="25">
+      <c r="D55" s="22">
         <v>32</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="22">
         <v>3.2</v>
       </c>
       <c r="F55" s="2">
@@ -7881,7 +7839,7 @@
       <c r="J55" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K55" s="26">
+      <c r="K55" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -7895,10 +7853,10 @@
       <c r="C56" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D56" s="25">
+      <c r="D56" s="22">
         <v>32</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="22">
         <v>3.2</v>
       </c>
       <c r="F56" s="2">
@@ -7916,7 +7874,7 @@
       <c r="J56" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K56" s="26">
+      <c r="K56" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -7930,10 +7888,10 @@
       <c r="C57" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D57" s="25">
+      <c r="D57" s="22">
         <v>32</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="22">
         <v>3.2</v>
       </c>
       <c r="F57" s="2">
@@ -7951,7 +7909,7 @@
       <c r="J57" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K57" s="26">
+      <c r="K57" s="23">
         <v>10517</v>
       </c>
     </row>
@@ -7965,10 +7923,10 @@
       <c r="C58" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D58" s="25">
+      <c r="D58" s="22">
         <v>32</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="22">
         <v>3.2</v>
       </c>
       <c r="F58" s="2">
@@ -7986,7 +7944,7 @@
       <c r="J58" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K58" s="26">
+      <c r="K58" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -8000,10 +7958,10 @@
       <c r="C59" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D59" s="25">
+      <c r="D59" s="22">
         <v>32</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="22">
         <v>3.2</v>
       </c>
       <c r="F59" s="2">
@@ -8021,7 +7979,7 @@
       <c r="J59" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K59" s="26">
+      <c r="K59" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8035,10 +7993,10 @@
       <c r="C60" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D60" s="25">
+      <c r="D60" s="22">
         <v>137</v>
       </c>
-      <c r="E60" s="25">
+      <c r="E60" s="22">
         <v>13.7</v>
       </c>
       <c r="F60" s="2">
@@ -8056,7 +8014,7 @@
       <c r="J60" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K60" s="26">
+      <c r="K60" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8070,10 +8028,10 @@
       <c r="C61" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D61" s="25">
+      <c r="D61" s="22">
         <v>137</v>
       </c>
-      <c r="E61" s="25">
+      <c r="E61" s="22">
         <v>13.7</v>
       </c>
       <c r="F61" s="2">
@@ -8091,7 +8049,7 @@
       <c r="J61" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K61" s="26">
+      <c r="K61" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8105,10 +8063,10 @@
       <c r="C62" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="D62" s="25">
+      <c r="D62" s="22">
         <v>109</v>
       </c>
-      <c r="E62" s="25">
+      <c r="E62" s="22">
         <v>10.9</v>
       </c>
       <c r="F62" s="2">
@@ -8126,7 +8084,7 @@
       <c r="J62" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K62" s="26">
+      <c r="K62" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8140,10 +8098,10 @@
       <c r="C63" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="D63" s="25">
+      <c r="D63" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E63" s="25">
+      <c r="E63" s="22">
         <v>7.89</v>
       </c>
       <c r="F63" s="2">
@@ -8161,7 +8119,7 @@
       <c r="J63" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K63" s="26">
+      <c r="K63" s="23">
         <v>12442</v>
       </c>
     </row>
@@ -8175,10 +8133,10 @@
       <c r="C64" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D64" s="25">
+      <c r="D64" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="22">
         <v>7.89</v>
       </c>
       <c r="F64" s="2">
@@ -8196,7 +8154,7 @@
       <c r="J64" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K64" s="26">
+      <c r="K64" s="23">
         <v>12442</v>
       </c>
     </row>
@@ -8210,10 +8168,10 @@
       <c r="C65" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="D65" s="25">
+      <c r="D65" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E65" s="25">
+      <c r="E65" s="22">
         <v>7.89</v>
       </c>
       <c r="F65" s="2">
@@ -8231,7 +8189,7 @@
       <c r="J65" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K65" s="26">
+      <c r="K65" s="23">
         <v>12442</v>
       </c>
     </row>
@@ -8245,10 +8203,10 @@
       <c r="C66" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="D66" s="25">
+      <c r="D66" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E66" s="25">
+      <c r="E66" s="22">
         <v>7.89</v>
       </c>
       <c r="F66" s="2">
@@ -8266,7 +8224,7 @@
       <c r="J66" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K66" s="26">
+      <c r="K66" s="23">
         <v>12442</v>
       </c>
     </row>
@@ -8280,10 +8238,10 @@
       <c r="C67" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="D67" s="25">
+      <c r="D67" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E67" s="25">
+      <c r="E67" s="22">
         <v>7.89</v>
       </c>
       <c r="F67" s="2">
@@ -8301,7 +8259,7 @@
       <c r="J67" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="K67" s="26">
+      <c r="K67" s="23">
         <v>9612</v>
       </c>
     </row>
@@ -8315,10 +8273,10 @@
       <c r="C68" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="D68" s="25">
+      <c r="D68" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E68" s="25">
+      <c r="E68" s="22">
         <v>7.89</v>
       </c>
       <c r="F68" s="2">
@@ -8336,7 +8294,7 @@
       <c r="J68" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K68" s="26">
+      <c r="K68" s="23">
         <v>11214</v>
       </c>
     </row>
@@ -8350,10 +8308,10 @@
       <c r="C69" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="D69" s="25">
+      <c r="D69" s="22">
         <v>169.66</v>
       </c>
-      <c r="E69" s="25">
+      <c r="E69" s="22">
         <v>16.97</v>
       </c>
       <c r="F69" s="2">
@@ -8371,7 +8329,7 @@
       <c r="J69" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K69" s="26">
+      <c r="K69" s="23">
         <v>11448</v>
       </c>
     </row>
@@ -8385,10 +8343,10 @@
       <c r="C70" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="D70" s="25">
+      <c r="D70" s="22">
         <v>132</v>
       </c>
-      <c r="E70" s="25">
+      <c r="E70" s="22">
         <v>13.2</v>
       </c>
       <c r="F70" s="2">
@@ -8406,7 +8364,7 @@
       <c r="J70" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K70" s="26">
+      <c r="K70" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8420,10 +8378,10 @@
       <c r="C71" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D71" s="25">
+      <c r="D71" s="22">
         <v>70</v>
       </c>
-      <c r="E71" s="25">
+      <c r="E71" s="22">
         <v>7</v>
       </c>
       <c r="F71" s="2">
@@ -8441,7 +8399,7 @@
       <c r="J71" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K71" s="26">
+      <c r="K71" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8455,10 +8413,10 @@
       <c r="C72" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="D72" s="25">
+      <c r="D72" s="22">
         <v>70</v>
       </c>
-      <c r="E72" s="25">
+      <c r="E72" s="22">
         <v>7</v>
       </c>
       <c r="F72" s="2">
@@ -8476,7 +8434,7 @@
       <c r="J72" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="K72" s="26">
+      <c r="K72" s="23">
         <v>18785</v>
       </c>
     </row>
@@ -8490,10 +8448,10 @@
       <c r="C73" s="2" t="s">
         <v>376</v>
       </c>
-      <c r="D73" s="25">
+      <c r="D73" s="22">
         <v>45</v>
       </c>
-      <c r="E73" s="25">
+      <c r="E73" s="22">
         <v>4.5</v>
       </c>
       <c r="F73" s="2">
@@ -8511,7 +8469,7 @@
       <c r="J73" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K73" s="26">
+      <c r="K73" s="23">
         <v>127</v>
       </c>
     </row>
@@ -8525,10 +8483,10 @@
       <c r="C74" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="D74" s="25">
+      <c r="D74" s="22">
         <v>184.9</v>
       </c>
-      <c r="E74" s="25">
+      <c r="E74" s="22">
         <v>18.489999999999998</v>
       </c>
       <c r="F74" s="2">
@@ -8546,7 +8504,7 @@
       <c r="J74" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K74" s="26">
+      <c r="K74" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8560,10 +8518,10 @@
       <c r="C75" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="D75" s="25">
+      <c r="D75" s="22">
         <v>162</v>
       </c>
-      <c r="E75" s="25">
+      <c r="E75" s="22">
         <v>16.2</v>
       </c>
       <c r="F75" s="2">
@@ -8581,7 +8539,7 @@
       <c r="J75" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K75" s="26">
+      <c r="K75" s="23">
         <v>506</v>
       </c>
     </row>
@@ -8595,10 +8553,10 @@
       <c r="C76" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D76" s="25">
+      <c r="D76" s="22">
         <v>184.9</v>
       </c>
-      <c r="E76" s="25">
+      <c r="E76" s="22">
         <v>0</v>
       </c>
       <c r="F76" s="2">
@@ -8616,7 +8574,7 @@
       <c r="J76" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K76" s="26">
+      <c r="K76" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -8630,10 +8588,10 @@
       <c r="C77" s="2" t="s">
         <v>379</v>
       </c>
-      <c r="D77" s="25">
+      <c r="D77" s="22">
         <v>184.9</v>
       </c>
-      <c r="E77" s="25">
+      <c r="E77" s="22">
         <v>18.489999999999998</v>
       </c>
       <c r="F77" s="2">
@@ -8651,7 +8609,7 @@
       <c r="J77" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K77" s="26">
+      <c r="K77" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -8665,10 +8623,10 @@
       <c r="C78" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="D78" s="25">
+      <c r="D78" s="22">
         <v>720</v>
       </c>
-      <c r="E78" s="25">
+      <c r="E78" s="22">
         <v>72</v>
       </c>
       <c r="F78" s="2">
@@ -8686,7 +8644,7 @@
       <c r="J78" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K78" s="26">
+      <c r="K78" s="23">
         <v>505</v>
       </c>
     </row>
@@ -8700,10 +8658,10 @@
       <c r="C79" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D79" s="25">
+      <c r="D79" s="22">
         <v>86.1</v>
       </c>
-      <c r="E79" s="25">
+      <c r="E79" s="22">
         <v>8.61</v>
       </c>
       <c r="F79" s="2">
@@ -8721,7 +8679,7 @@
       <c r="J79" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K79" s="26">
+      <c r="K79" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -8735,10 +8693,10 @@
       <c r="C80" s="2" t="s">
         <v>381</v>
       </c>
-      <c r="D80" s="25">
+      <c r="D80" s="22">
         <v>86.1</v>
       </c>
-      <c r="E80" s="25">
+      <c r="E80" s="22">
         <v>8.61</v>
       </c>
       <c r="F80" s="2">
@@ -8756,7 +8714,7 @@
       <c r="J80" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K80" s="26">
+      <c r="K80" s="23">
         <v>9698</v>
       </c>
     </row>
@@ -8770,10 +8728,10 @@
       <c r="C81" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D81" s="25">
+      <c r="D81" s="22">
         <v>90</v>
       </c>
-      <c r="E81" s="25">
+      <c r="E81" s="22">
         <v>9</v>
       </c>
       <c r="F81" s="2">
@@ -8791,7 +8749,7 @@
       <c r="J81" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K81" s="26">
+      <c r="K81" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -8805,10 +8763,10 @@
       <c r="C82" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D82" s="25">
+      <c r="D82" s="22">
         <v>90</v>
       </c>
-      <c r="E82" s="25">
+      <c r="E82" s="22">
         <v>9</v>
       </c>
       <c r="F82" s="2">
@@ -8826,7 +8784,7 @@
       <c r="J82" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K82" s="26">
+      <c r="K82" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -8840,10 +8798,10 @@
       <c r="C83" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="D83" s="25">
+      <c r="D83" s="22">
         <v>114.55</v>
       </c>
-      <c r="E83" s="25">
+      <c r="E83" s="22">
         <v>11.46</v>
       </c>
       <c r="F83" s="2">
@@ -8861,7 +8819,7 @@
       <c r="J83" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K83" s="26">
+      <c r="K83" s="23">
         <v>11448</v>
       </c>
     </row>
@@ -8875,10 +8833,10 @@
       <c r="C84" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D84" s="25">
+      <c r="D84" s="22">
         <v>110</v>
       </c>
-      <c r="E84" s="25">
+      <c r="E84" s="22">
         <v>11</v>
       </c>
       <c r="F84" s="2">
@@ -8896,7 +8854,7 @@
       <c r="J84" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K84" s="26">
+      <c r="K84" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -8910,10 +8868,10 @@
       <c r="C85" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="D85" s="25">
+      <c r="D85" s="22">
         <v>110</v>
       </c>
-      <c r="E85" s="25">
+      <c r="E85" s="22">
         <v>11</v>
       </c>
       <c r="F85" s="2">
@@ -8931,7 +8889,7 @@
       <c r="J85" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K85" s="26">
+      <c r="K85" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -8945,10 +8903,10 @@
       <c r="C86" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D86" s="25">
+      <c r="D86" s="22">
         <v>64.75</v>
       </c>
-      <c r="E86" s="25">
+      <c r="E86" s="22">
         <v>6.48</v>
       </c>
       <c r="F86" s="2">
@@ -8966,7 +8924,7 @@
       <c r="J86" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K86" s="26">
+      <c r="K86" s="23">
         <v>11214</v>
       </c>
     </row>
@@ -8980,10 +8938,10 @@
       <c r="C87" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D87" s="25">
+      <c r="D87" s="22">
         <v>64.75</v>
       </c>
-      <c r="E87" s="25">
+      <c r="E87" s="22">
         <v>6.48</v>
       </c>
       <c r="F87" s="2">
@@ -9001,7 +8959,7 @@
       <c r="J87" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="K87" s="26">
+      <c r="K87" s="23">
         <v>12442</v>
       </c>
     </row>
@@ -9015,10 +8973,10 @@
       <c r="C88" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="D88" s="25">
+      <c r="D88" s="22">
         <v>64.75</v>
       </c>
-      <c r="E88" s="25">
+      <c r="E88" s="22">
         <v>6.48</v>
       </c>
       <c r="F88" s="2">
@@ -9036,7 +8994,7 @@
       <c r="J88" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K88" s="26">
+      <c r="K88" s="23">
         <v>11214</v>
       </c>
     </row>
@@ -9050,10 +9008,10 @@
       <c r="C89" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D89" s="25">
+      <c r="D89" s="22">
         <v>68</v>
       </c>
-      <c r="E89" s="25">
+      <c r="E89" s="22">
         <v>6.8</v>
       </c>
       <c r="F89" s="2">
@@ -9071,7 +9029,7 @@
       <c r="J89" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K89" s="26">
+      <c r="K89" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -9085,10 +9043,10 @@
       <c r="C90" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="D90" s="25">
+      <c r="D90" s="22">
         <v>68</v>
       </c>
-      <c r="E90" s="25">
+      <c r="E90" s="22">
         <v>6.8</v>
       </c>
       <c r="F90" s="2">
@@ -9106,7 +9064,7 @@
       <c r="J90" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K90" s="26">
+      <c r="K90" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -9120,10 +9078,10 @@
       <c r="C91" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D91" s="25">
+      <c r="D91" s="22">
         <v>93</v>
       </c>
-      <c r="E91" s="25">
+      <c r="E91" s="22">
         <v>9.3000000000000007</v>
       </c>
       <c r="F91" s="2">
@@ -9141,7 +9099,7 @@
       <c r="J91" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K91" s="26">
+      <c r="K91" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -9155,10 +9113,10 @@
       <c r="C92" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D92" s="25">
+      <c r="D92" s="22">
         <v>93</v>
       </c>
-      <c r="E92" s="25">
+      <c r="E92" s="22">
         <v>0</v>
       </c>
       <c r="F92" s="2">
@@ -9176,7 +9134,7 @@
       <c r="J92" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K92" s="26">
+      <c r="K92" s="23">
         <v>9698</v>
       </c>
     </row>
@@ -9190,10 +9148,10 @@
       <c r="C93" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D93" s="25">
+      <c r="D93" s="22">
         <v>93</v>
       </c>
-      <c r="E93" s="25">
+      <c r="E93" s="22">
         <v>9.3000000000000007</v>
       </c>
       <c r="F93" s="2">
@@ -9211,7 +9169,7 @@
       <c r="J93" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K93" s="26">
+      <c r="K93" s="23">
         <v>504</v>
       </c>
     </row>
@@ -9225,10 +9183,10 @@
       <c r="C94" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D94" s="25">
+      <c r="D94" s="22">
         <v>93</v>
       </c>
-      <c r="E94" s="25">
+      <c r="E94" s="22">
         <v>9.3000000000000007</v>
       </c>
       <c r="F94" s="2">
@@ -9246,7 +9204,7 @@
       <c r="J94" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K94" s="26">
+      <c r="K94" s="23">
         <v>504</v>
       </c>
     </row>
@@ -9260,10 +9218,10 @@
       <c r="C95" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="D95" s="25">
+      <c r="D95" s="22">
         <v>2170</v>
       </c>
-      <c r="E95" s="25">
+      <c r="E95" s="22">
         <v>217</v>
       </c>
       <c r="F95" s="2">
@@ -9281,7 +9239,7 @@
       <c r="J95" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K95" s="26">
+      <c r="K95" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -9295,10 +9253,10 @@
       <c r="C96" s="2" t="s">
         <v>389</v>
       </c>
-      <c r="D96" s="25">
+      <c r="D96" s="22">
         <v>547.04999999999995</v>
       </c>
-      <c r="E96" s="25">
+      <c r="E96" s="22">
         <v>54.71</v>
       </c>
       <c r="F96" s="2">
@@ -9316,7 +9274,7 @@
       <c r="J96" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="K96" s="26">
+      <c r="K96" s="23">
         <v>11448</v>
       </c>
     </row>
@@ -9330,10 +9288,10 @@
       <c r="C97" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D97" s="25">
+      <c r="D97" s="22">
         <v>125</v>
       </c>
-      <c r="E97" s="25">
+      <c r="E97" s="22">
         <v>12.5</v>
       </c>
       <c r="F97" s="2">
@@ -9351,7 +9309,7 @@
       <c r="J97" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K97" s="26">
+      <c r="K97" s="23">
         <v>13744</v>
       </c>
     </row>
@@ -9365,10 +9323,10 @@
       <c r="C98" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D98" s="25">
+      <c r="D98" s="22">
         <v>185</v>
       </c>
-      <c r="E98" s="25">
+      <c r="E98" s="22">
         <v>18.5</v>
       </c>
       <c r="F98" s="2">
@@ -9386,7 +9344,7 @@
       <c r="J98" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="K98" s="26">
+      <c r="K98" s="23">
         <v>1373</v>
       </c>
     </row>
@@ -9400,10 +9358,10 @@
       <c r="C99" s="2" t="s">
         <v>390</v>
       </c>
-      <c r="D99" s="25">
+      <c r="D99" s="22">
         <v>169</v>
       </c>
-      <c r="E99" s="25">
+      <c r="E99" s="22">
         <v>16.899999999999999</v>
       </c>
       <c r="F99" s="2">
@@ -9421,7 +9379,7 @@
       <c r="J99" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K99" s="26">
+      <c r="K99" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -9435,10 +9393,10 @@
       <c r="C100" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D100" s="25">
+      <c r="D100" s="22">
         <v>1150</v>
       </c>
-      <c r="E100" s="25">
+      <c r="E100" s="22">
         <v>115</v>
       </c>
       <c r="F100" s="2">
@@ -9456,7 +9414,7 @@
       <c r="J100" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="K100" s="26">
+      <c r="K100" s="23">
         <v>12443</v>
       </c>
     </row>
@@ -9470,10 +9428,10 @@
       <c r="C101" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="D101" s="25">
+      <c r="D101" s="22">
         <v>1371</v>
       </c>
-      <c r="E101" s="25">
+      <c r="E101" s="22">
         <v>137.1</v>
       </c>
       <c r="F101" s="2">
@@ -9491,7 +9449,7 @@
       <c r="J101" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="K101" s="26">
+      <c r="K101" s="23">
         <v>12443</v>
       </c>
     </row>
@@ -9505,10 +9463,10 @@
       <c r="C102" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="D102" s="25">
+      <c r="D102" s="22">
         <v>550</v>
       </c>
-      <c r="E102" s="25">
+      <c r="E102" s="22">
         <v>55</v>
       </c>
       <c r="F102" s="2">
@@ -9526,7 +9484,7 @@
       <c r="J102" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K102" s="26">
+      <c r="K102" s="23">
         <v>506</v>
       </c>
     </row>
@@ -9540,10 +9498,10 @@
       <c r="C103" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D103" s="25">
+      <c r="D103" s="22">
         <v>182.84</v>
       </c>
-      <c r="E103" s="25">
+      <c r="E103" s="22">
         <v>18.28</v>
       </c>
       <c r="F103" s="2">
@@ -9561,7 +9519,7 @@
       <c r="J103" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K103" s="26">
+      <c r="K103" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -9575,10 +9533,10 @@
       <c r="C104" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="D104" s="25">
+      <c r="D104" s="22">
         <v>756.25</v>
       </c>
-      <c r="E104" s="25">
+      <c r="E104" s="22">
         <v>75.63</v>
       </c>
       <c r="F104" s="2">
@@ -9596,7 +9554,7 @@
       <c r="J104" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="K104" s="26">
+      <c r="K104" s="23">
         <v>12443</v>
       </c>
     </row>
@@ -9610,10 +9568,10 @@
       <c r="C105" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D105" s="25">
+      <c r="D105" s="22">
         <v>190</v>
       </c>
-      <c r="E105" s="25">
+      <c r="E105" s="22">
         <v>19</v>
       </c>
       <c r="F105" s="2">
@@ -9631,7 +9589,7 @@
       <c r="J105" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K105" s="26">
+      <c r="K105" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -9645,10 +9603,10 @@
       <c r="C106" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D106" s="25">
+      <c r="D106" s="22">
         <v>119.98</v>
       </c>
-      <c r="E106" s="25">
+      <c r="E106" s="22">
         <v>12</v>
       </c>
       <c r="F106" s="2">
@@ -9666,7 +9624,7 @@
       <c r="J106" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K106" s="26">
+      <c r="K106" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -9680,10 +9638,10 @@
       <c r="C107" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D107" s="25">
+      <c r="D107" s="22">
         <v>190</v>
       </c>
-      <c r="E107" s="25">
+      <c r="E107" s="22">
         <v>19</v>
       </c>
       <c r="F107" s="2">
@@ -9701,7 +9659,7 @@
       <c r="J107" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K107" s="26">
+      <c r="K107" s="23">
         <v>504</v>
       </c>
     </row>
@@ -9715,10 +9673,10 @@
       <c r="C108" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="D108" s="25">
+      <c r="D108" s="22">
         <v>142.86000000000001</v>
       </c>
-      <c r="E108" s="25">
+      <c r="E108" s="22">
         <v>14.29</v>
       </c>
       <c r="F108" s="2">
@@ -9736,7 +9694,7 @@
       <c r="J108" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K108" s="26">
+      <c r="K108" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -9750,10 +9708,10 @@
       <c r="C109" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D109" s="25">
+      <c r="D109" s="22">
         <v>500</v>
       </c>
-      <c r="E109" s="25">
+      <c r="E109" s="22">
         <v>50</v>
       </c>
       <c r="F109" s="2">
@@ -9771,7 +9729,7 @@
       <c r="J109" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K109" s="26">
+      <c r="K109" s="23">
         <v>11213</v>
       </c>
     </row>
@@ -9785,10 +9743,10 @@
       <c r="C110" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D110" s="25">
+      <c r="D110" s="22">
         <v>206</v>
       </c>
-      <c r="E110" s="25">
+      <c r="E110" s="22">
         <v>20.6</v>
       </c>
       <c r="F110" s="2">
@@ -9806,7 +9764,7 @@
       <c r="J110" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K110" s="26">
+      <c r="K110" s="23">
         <v>13744</v>
       </c>
     </row>
@@ -9820,10 +9778,10 @@
       <c r="C111" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D111" s="25">
+      <c r="D111" s="22">
         <v>185</v>
       </c>
-      <c r="E111" s="25">
+      <c r="E111" s="22">
         <v>18.5</v>
       </c>
       <c r="F111" s="2">
@@ -9841,7 +9799,7 @@
       <c r="J111" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K111" s="26">
+      <c r="K111" s="23">
         <v>504</v>
       </c>
     </row>
@@ -9855,10 +9813,10 @@
       <c r="C112" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D112" s="25">
+      <c r="D112" s="22">
         <v>185</v>
       </c>
-      <c r="E112" s="25">
+      <c r="E112" s="22">
         <v>18.5</v>
       </c>
       <c r="F112" s="2">
@@ -9876,7 +9834,7 @@
       <c r="J112" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K112" s="26">
+      <c r="K112" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -9890,10 +9848,10 @@
       <c r="C113" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D113" s="25">
+      <c r="D113" s="22">
         <v>185</v>
       </c>
-      <c r="E113" s="25">
+      <c r="E113" s="22">
         <v>18.5</v>
       </c>
       <c r="F113" s="2">
@@ -9911,7 +9869,7 @@
       <c r="J113" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K113" s="26">
+      <c r="K113" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -9925,10 +9883,10 @@
       <c r="C114" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D114" s="25">
+      <c r="D114" s="22">
         <v>185</v>
       </c>
-      <c r="E114" s="25">
+      <c r="E114" s="22">
         <v>18.5</v>
       </c>
       <c r="F114" s="2">
@@ -9946,7 +9904,7 @@
       <c r="J114" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K114" s="26">
+      <c r="K114" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -9960,10 +9918,10 @@
       <c r="C115" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D115" s="25">
+      <c r="D115" s="22">
         <v>185</v>
       </c>
-      <c r="E115" s="25">
+      <c r="E115" s="22">
         <v>18.5</v>
       </c>
       <c r="F115" s="2">
@@ -9981,7 +9939,7 @@
       <c r="J115" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K115" s="26">
+      <c r="K115" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -9995,10 +9953,10 @@
       <c r="C116" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="D116" s="25">
+      <c r="D116" s="22">
         <v>619</v>
       </c>
-      <c r="E116" s="25">
+      <c r="E116" s="22">
         <v>61.9</v>
       </c>
       <c r="F116" s="2">
@@ -10016,7 +9974,7 @@
       <c r="J116" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="K116" s="26">
+      <c r="K116" s="23">
         <v>12443</v>
       </c>
     </row>
@@ -10030,10 +9988,10 @@
       <c r="C117" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="D117" s="25">
+      <c r="D117" s="22">
         <v>480.1</v>
       </c>
-      <c r="E117" s="25">
+      <c r="E117" s="22">
         <v>48.01</v>
       </c>
       <c r="F117" s="2">
@@ -10051,7 +10009,7 @@
       <c r="J117" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K117" s="26">
+      <c r="K117" s="23">
         <v>953</v>
       </c>
     </row>
@@ -10065,10 +10023,10 @@
       <c r="C118" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D118" s="25">
+      <c r="D118" s="22">
         <v>340</v>
       </c>
-      <c r="E118" s="25">
+      <c r="E118" s="22">
         <v>34</v>
       </c>
       <c r="F118" s="2">
@@ -10086,7 +10044,7 @@
       <c r="J118" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K118" s="26">
+      <c r="K118" s="23">
         <v>953</v>
       </c>
     </row>
@@ -10100,10 +10058,10 @@
       <c r="C119" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="D119" s="25">
+      <c r="D119" s="22">
         <v>316.60000000000002</v>
       </c>
-      <c r="E119" s="25">
+      <c r="E119" s="22">
         <v>31.66</v>
       </c>
       <c r="F119" s="2">
@@ -10121,7 +10079,7 @@
       <c r="J119" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K119" s="26">
+      <c r="K119" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -10135,10 +10093,10 @@
       <c r="C120" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="D120" s="25">
+      <c r="D120" s="22">
         <v>448</v>
       </c>
-      <c r="E120" s="25">
+      <c r="E120" s="22">
         <v>44.8</v>
       </c>
       <c r="F120" s="2">
@@ -10156,7 +10114,7 @@
       <c r="J120" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K120" s="26">
+      <c r="K120" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10170,10 +10128,10 @@
       <c r="C121" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D121" s="25">
+      <c r="D121" s="22">
         <v>134</v>
       </c>
-      <c r="E121" s="25">
+      <c r="E121" s="22">
         <v>13.4</v>
       </c>
       <c r="F121" s="2">
@@ -10191,7 +10149,7 @@
       <c r="J121" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K121" s="26">
+      <c r="K121" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10205,10 +10163,10 @@
       <c r="C122" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="D122" s="25">
+      <c r="D122" s="22">
         <v>134</v>
       </c>
-      <c r="E122" s="25">
+      <c r="E122" s="22">
         <v>13.4</v>
       </c>
       <c r="F122" s="2">
@@ -10226,7 +10184,7 @@
       <c r="J122" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K122" s="26">
+      <c r="K122" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10240,10 +10198,10 @@
       <c r="C123" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="D123" s="25">
+      <c r="D123" s="22">
         <v>370.27</v>
       </c>
-      <c r="E123" s="25">
+      <c r="E123" s="22">
         <v>37.03</v>
       </c>
       <c r="F123" s="2">
@@ -10261,7 +10219,7 @@
       <c r="J123" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K123" s="26">
+      <c r="K123" s="23">
         <v>953</v>
       </c>
     </row>
@@ -10275,10 +10233,10 @@
       <c r="C124" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="D124" s="25">
+      <c r="D124" s="22">
         <v>500</v>
       </c>
-      <c r="E124" s="25">
+      <c r="E124" s="22">
         <v>50</v>
       </c>
       <c r="F124" s="2">
@@ -10296,7 +10254,7 @@
       <c r="J124" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K124" s="26">
+      <c r="K124" s="23">
         <v>953</v>
       </c>
     </row>
@@ -10310,10 +10268,10 @@
       <c r="C125" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D125" s="25">
+      <c r="D125" s="22">
         <v>238</v>
       </c>
-      <c r="E125" s="25">
+      <c r="E125" s="22">
         <v>23.8</v>
       </c>
       <c r="F125" s="2">
@@ -10331,7 +10289,7 @@
       <c r="J125" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K125" s="26">
+      <c r="K125" s="23">
         <v>11214</v>
       </c>
     </row>
@@ -10345,10 +10303,10 @@
       <c r="C126" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D126" s="25">
+      <c r="D126" s="22">
         <v>195</v>
       </c>
-      <c r="E126" s="25">
+      <c r="E126" s="22">
         <v>19.5</v>
       </c>
       <c r="F126" s="2">
@@ -10366,7 +10324,7 @@
       <c r="J126" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K126" s="26">
+      <c r="K126" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -10380,10 +10338,10 @@
       <c r="C127" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D127" s="25">
+      <c r="D127" s="22">
         <v>130</v>
       </c>
-      <c r="E127" s="25">
+      <c r="E127" s="22">
         <v>13</v>
       </c>
       <c r="F127" s="2">
@@ -10401,7 +10359,7 @@
       <c r="J127" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K127" s="26">
+      <c r="K127" s="23">
         <v>505</v>
       </c>
     </row>
@@ -10415,10 +10373,10 @@
       <c r="C128" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D128" s="25">
+      <c r="D128" s="22">
         <v>195</v>
       </c>
-      <c r="E128" s="25">
+      <c r="E128" s="22">
         <v>19.5</v>
       </c>
       <c r="F128" s="2">
@@ -10436,7 +10394,7 @@
       <c r="J128" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K128" s="26">
+      <c r="K128" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10450,10 +10408,10 @@
       <c r="C129" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="D129" s="25">
+      <c r="D129" s="22">
         <v>725.24</v>
       </c>
-      <c r="E129" s="25">
+      <c r="E129" s="22">
         <v>72.52</v>
       </c>
       <c r="F129" s="2">
@@ -10471,7 +10429,7 @@
       <c r="J129" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="K129" s="26">
+      <c r="K129" s="23">
         <v>12441</v>
       </c>
     </row>
@@ -10485,10 +10443,10 @@
       <c r="C130" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D130" s="25">
+      <c r="D130" s="22">
         <v>450</v>
       </c>
-      <c r="E130" s="25">
+      <c r="E130" s="22">
         <v>45</v>
       </c>
       <c r="F130" s="2">
@@ -10506,7 +10464,7 @@
       <c r="J130" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K130" s="26">
+      <c r="K130" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10520,10 +10478,10 @@
       <c r="C131" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="D131" s="25">
+      <c r="D131" s="22">
         <v>450</v>
       </c>
-      <c r="E131" s="25">
+      <c r="E131" s="22">
         <v>45</v>
       </c>
       <c r="F131" s="2">
@@ -10541,7 +10499,7 @@
       <c r="J131" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K131" s="26">
+      <c r="K131" s="23">
         <v>27049</v>
       </c>
     </row>
@@ -10555,10 +10513,10 @@
       <c r="C132" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="D132" s="25">
+      <c r="D132" s="22">
         <v>350</v>
       </c>
-      <c r="E132" s="25">
+      <c r="E132" s="22">
         <v>35</v>
       </c>
       <c r="F132" s="2">
@@ -10576,7 +10534,7 @@
       <c r="J132" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="K132" s="26">
+      <c r="K132" s="23">
         <v>11535</v>
       </c>
     </row>
@@ -10590,10 +10548,10 @@
       <c r="C133" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="D133" s="25">
+      <c r="D133" s="22">
         <v>900</v>
       </c>
-      <c r="E133" s="25">
+      <c r="E133" s="22">
         <v>90</v>
       </c>
       <c r="F133" s="2">
@@ -10611,7 +10569,7 @@
       <c r="J133" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K133" s="26">
+      <c r="K133" s="23">
         <v>11216</v>
       </c>
     </row>
@@ -10625,10 +10583,10 @@
       <c r="C134" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="D134" s="25">
+      <c r="D134" s="22">
         <v>400</v>
       </c>
-      <c r="E134" s="25">
+      <c r="E134" s="22">
         <v>40</v>
       </c>
       <c r="F134" s="2">
@@ -10646,7 +10604,7 @@
       <c r="J134" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K134" s="26">
+      <c r="K134" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -10660,10 +10618,10 @@
       <c r="C135" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D135" s="25">
+      <c r="D135" s="22">
         <v>450</v>
       </c>
-      <c r="E135" s="25">
+      <c r="E135" s="22">
         <v>45</v>
       </c>
       <c r="F135" s="2">
@@ -10681,7 +10639,7 @@
       <c r="J135" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K135" s="26">
+      <c r="K135" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -10695,10 +10653,10 @@
       <c r="C136" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D136" s="25">
+      <c r="D136" s="22">
         <v>450</v>
       </c>
-      <c r="E136" s="25">
+      <c r="E136" s="22">
         <v>45</v>
       </c>
       <c r="F136" s="2">
@@ -10716,7 +10674,7 @@
       <c r="J136" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K136" s="26">
+      <c r="K136" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -10730,10 +10688,10 @@
       <c r="C137" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D137" s="25">
+      <c r="D137" s="22">
         <v>562.07000000000005</v>
       </c>
-      <c r="E137" s="25">
+      <c r="E137" s="22">
         <v>56.21</v>
       </c>
       <c r="F137" s="2">
@@ -10751,7 +10709,7 @@
       <c r="J137" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K137" s="26">
+      <c r="K137" s="23">
         <v>11216</v>
       </c>
     </row>
@@ -10765,10 +10723,10 @@
       <c r="C138" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="D138" s="25">
+      <c r="D138" s="22">
         <v>545</v>
       </c>
-      <c r="E138" s="25">
+      <c r="E138" s="22">
         <v>54.5</v>
       </c>
       <c r="F138" s="2">
@@ -10786,7 +10744,7 @@
       <c r="J138" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="K138" s="26">
+      <c r="K138" s="23">
         <v>1373</v>
       </c>
     </row>
@@ -10800,10 +10758,10 @@
       <c r="C139" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="D139" s="25">
+      <c r="D139" s="22">
         <v>571.91999999999996</v>
       </c>
-      <c r="E139" s="25">
+      <c r="E139" s="22">
         <v>57.19</v>
       </c>
       <c r="F139" s="2">
@@ -10821,7 +10779,7 @@
       <c r="J139" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K139" s="26">
+      <c r="K139" s="23">
         <v>27049</v>
       </c>
     </row>
@@ -10835,10 +10793,10 @@
       <c r="C140" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D140" s="25">
+      <c r="D140" s="22">
         <v>221</v>
       </c>
-      <c r="E140" s="25">
+      <c r="E140" s="22">
         <v>22.1</v>
       </c>
       <c r="F140" s="2">
@@ -10856,7 +10814,7 @@
       <c r="J140" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K140" s="26">
+      <c r="K140" s="23">
         <v>504</v>
       </c>
     </row>
@@ -10870,10 +10828,10 @@
       <c r="C141" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D141" s="25">
+      <c r="D141" s="22">
         <v>221</v>
       </c>
-      <c r="E141" s="25">
+      <c r="E141" s="22">
         <v>22.1</v>
       </c>
       <c r="F141" s="2">
@@ -10891,7 +10849,7 @@
       <c r="J141" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K141" s="26">
+      <c r="K141" s="23">
         <v>505</v>
       </c>
     </row>
@@ -10905,10 +10863,10 @@
       <c r="C142" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D142" s="25">
+      <c r="D142" s="22">
         <v>211</v>
       </c>
-      <c r="E142" s="25">
+      <c r="E142" s="22">
         <v>21.1</v>
       </c>
       <c r="F142" s="2">
@@ -10926,7 +10884,7 @@
       <c r="J142" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K142" s="26">
+      <c r="K142" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -10940,10 +10898,10 @@
       <c r="C143" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="D143" s="25">
+      <c r="D143" s="22">
         <v>1282</v>
       </c>
-      <c r="E143" s="25">
+      <c r="E143" s="22">
         <v>128.19999999999999</v>
       </c>
       <c r="F143" s="2">
@@ -10961,7 +10919,7 @@
       <c r="J143" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K143" s="26">
+      <c r="K143" s="23">
         <v>953</v>
       </c>
     </row>
@@ -10975,10 +10933,10 @@
       <c r="C144" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D144" s="25">
+      <c r="D144" s="22">
         <v>211</v>
       </c>
-      <c r="E144" s="25">
+      <c r="E144" s="22">
         <v>21.1</v>
       </c>
       <c r="F144" s="2">
@@ -10996,7 +10954,7 @@
       <c r="J144" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K144" s="26">
+      <c r="K144" s="23">
         <v>953</v>
       </c>
     </row>
@@ -11010,10 +10968,10 @@
       <c r="C145" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D145" s="25">
+      <c r="D145" s="22">
         <v>211</v>
       </c>
-      <c r="E145" s="25">
+      <c r="E145" s="22">
         <v>21.1</v>
       </c>
       <c r="F145" s="2">
@@ -11031,7 +10989,7 @@
       <c r="J145" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K145" s="26">
+      <c r="K145" s="23">
         <v>953</v>
       </c>
     </row>
@@ -11045,10 +11003,10 @@
       <c r="C146" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="D146" s="25">
+      <c r="D146" s="22">
         <v>1720.01</v>
       </c>
-      <c r="E146" s="25">
+      <c r="E146" s="22">
         <v>172</v>
       </c>
       <c r="F146" s="2">
@@ -11066,7 +11024,7 @@
       <c r="J146" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K146" s="26">
+      <c r="K146" s="23">
         <v>9698</v>
       </c>
     </row>
@@ -11080,10 +11038,10 @@
       <c r="C147" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="D147" s="25">
+      <c r="D147" s="22">
         <v>351.99</v>
       </c>
-      <c r="E147" s="25">
+      <c r="E147" s="22">
         <v>35.200000000000003</v>
       </c>
       <c r="F147" s="2">
@@ -11101,7 +11059,7 @@
       <c r="J147" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K147" s="26">
+      <c r="K147" s="23">
         <v>11217</v>
       </c>
     </row>
@@ -11115,10 +11073,10 @@
       <c r="C148" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D148" s="25">
+      <c r="D148" s="22">
         <v>307</v>
       </c>
-      <c r="E148" s="25">
+      <c r="E148" s="22">
         <v>30.7</v>
       </c>
       <c r="F148" s="2">
@@ -11136,7 +11094,7 @@
       <c r="J148" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="K148" s="26">
+      <c r="K148" s="23">
         <v>26537</v>
       </c>
     </row>
@@ -11150,10 +11108,10 @@
       <c r="C149" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="D149" s="25">
+      <c r="D149" s="22">
         <v>3120</v>
       </c>
-      <c r="E149" s="25">
+      <c r="E149" s="22">
         <v>312</v>
       </c>
       <c r="F149" s="2">
@@ -11171,7 +11129,7 @@
       <c r="J149" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K149" s="26">
+      <c r="K149" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11185,10 +11143,10 @@
       <c r="C150" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="D150" s="25">
+      <c r="D150" s="22">
         <v>5100</v>
       </c>
-      <c r="E150" s="25">
+      <c r="E150" s="22">
         <v>510</v>
       </c>
       <c r="F150" s="2">
@@ -11206,7 +11164,7 @@
       <c r="J150" s="2" t="s">
         <v>358</v>
       </c>
-      <c r="K150" s="26">
+      <c r="K150" s="23">
         <v>13744</v>
       </c>
     </row>
@@ -11220,10 +11178,10 @@
       <c r="C151" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D151" s="25">
+      <c r="D151" s="22">
         <v>367</v>
       </c>
-      <c r="E151" s="25">
+      <c r="E151" s="22">
         <v>36.700000000000003</v>
       </c>
       <c r="F151" s="2">
@@ -11241,7 +11199,7 @@
       <c r="J151" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K151" s="26">
+      <c r="K151" s="23">
         <v>953</v>
       </c>
     </row>
@@ -11255,10 +11213,10 @@
       <c r="C152" s="2" t="s">
         <v>421</v>
       </c>
-      <c r="D152" s="25">
+      <c r="D152" s="22">
         <v>609.99</v>
       </c>
-      <c r="E152" s="25">
+      <c r="E152" s="22">
         <v>61</v>
       </c>
       <c r="F152" s="2">
@@ -11276,7 +11234,7 @@
       <c r="J152" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K152" s="26">
+      <c r="K152" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11290,10 +11248,10 @@
       <c r="C153" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="D153" s="25">
+      <c r="D153" s="22">
         <v>600</v>
       </c>
-      <c r="E153" s="25">
+      <c r="E153" s="22">
         <v>60</v>
       </c>
       <c r="F153" s="2">
@@ -11311,7 +11269,7 @@
       <c r="J153" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K153" s="26">
+      <c r="K153" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -11325,10 +11283,10 @@
       <c r="C154" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="D154" s="25">
+      <c r="D154" s="22">
         <v>349</v>
       </c>
-      <c r="E154" s="25">
+      <c r="E154" s="22">
         <v>34.9</v>
       </c>
       <c r="F154" s="2">
@@ -11346,7 +11304,7 @@
       <c r="J154" s="2" t="s">
         <v>371</v>
       </c>
-      <c r="K154" s="26">
+      <c r="K154" s="23">
         <v>11214</v>
       </c>
     </row>
@@ -11360,10 +11318,10 @@
       <c r="C155" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D155" s="25">
+      <c r="D155" s="22">
         <v>365.25</v>
       </c>
-      <c r="E155" s="25">
+      <c r="E155" s="22">
         <v>36.53</v>
       </c>
       <c r="F155" s="2">
@@ -11381,7 +11339,7 @@
       <c r="J155" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="K155" s="26">
+      <c r="K155" s="23">
         <v>9509</v>
       </c>
     </row>
@@ -11395,10 +11353,10 @@
       <c r="C156" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D156" s="25">
+      <c r="D156" s="22">
         <v>365.25</v>
       </c>
-      <c r="E156" s="25">
+      <c r="E156" s="22">
         <v>160.5</v>
       </c>
       <c r="F156" s="2">
@@ -11416,7 +11374,7 @@
       <c r="J156" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K156" s="26">
+      <c r="K156" s="23">
         <v>29329</v>
       </c>
     </row>
@@ -11430,10 +11388,10 @@
       <c r="C157" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D157" s="25">
+      <c r="D157" s="22">
         <v>298.85000000000002</v>
       </c>
-      <c r="E157" s="25">
+      <c r="E157" s="22">
         <v>142.05000000000001</v>
       </c>
       <c r="F157" s="2">
@@ -11451,7 +11409,7 @@
       <c r="J157" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="K157" s="26">
+      <c r="K157" s="23">
         <v>19423</v>
       </c>
     </row>
@@ -11465,10 +11423,10 @@
       <c r="C158" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D158" s="25">
+      <c r="D158" s="22">
         <v>298.85000000000002</v>
       </c>
-      <c r="E158" s="25">
+      <c r="E158" s="22">
         <v>142.05000000000001</v>
       </c>
       <c r="F158" s="2">
@@ -11486,7 +11444,7 @@
       <c r="J158" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K158" s="26">
+      <c r="K158" s="23">
         <v>19422</v>
       </c>
     </row>
@@ -11500,10 +11458,10 @@
       <c r="C159" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="D159" s="25">
+      <c r="D159" s="22">
         <v>1318.8</v>
       </c>
-      <c r="E159" s="25">
+      <c r="E159" s="22">
         <v>626.5</v>
       </c>
       <c r="F159" s="2">
@@ -11521,7 +11479,7 @@
       <c r="J159" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="K159" s="26">
+      <c r="K159" s="23">
         <v>19423</v>
       </c>
     </row>
@@ -11535,10 +11493,10 @@
       <c r="C160" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="D160" s="25">
+      <c r="D160" s="22">
         <v>420</v>
       </c>
-      <c r="E160" s="25">
+      <c r="E160" s="22">
         <v>237.3</v>
       </c>
       <c r="F160" s="2">
@@ -11556,7 +11514,7 @@
       <c r="J160" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="K160" s="26">
+      <c r="K160" s="23">
         <v>11061</v>
       </c>
     </row>
@@ -11570,10 +11528,10 @@
       <c r="C161" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D161" s="25">
+      <c r="D161" s="22">
         <v>593.27</v>
       </c>
-      <c r="E161" s="25">
+      <c r="E161" s="22">
         <v>353.51</v>
       </c>
       <c r="F161" s="2">
@@ -11591,7 +11549,7 @@
       <c r="J161" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K161" s="26">
+      <c r="K161" s="23">
         <v>1082</v>
       </c>
     </row>
@@ -11605,10 +11563,10 @@
       <c r="C162" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D162" s="25">
+      <c r="D162" s="22">
         <v>593.27</v>
       </c>
-      <c r="E162" s="25">
+      <c r="E162" s="22">
         <v>353.51</v>
       </c>
       <c r="F162" s="2">
@@ -11626,7 +11584,7 @@
       <c r="J162" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K162" s="26">
+      <c r="K162" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11640,10 +11598,10 @@
       <c r="C163" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D163" s="25">
+      <c r="D163" s="22">
         <v>593.27</v>
       </c>
-      <c r="E163" s="25">
+      <c r="E163" s="22">
         <v>353.51</v>
       </c>
       <c r="F163" s="2">
@@ -11661,7 +11619,7 @@
       <c r="J163" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K163" s="26">
+      <c r="K163" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11675,10 +11633,10 @@
       <c r="C164" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D164" s="25">
+      <c r="D164" s="22">
         <v>593.27</v>
       </c>
-      <c r="E164" s="25">
+      <c r="E164" s="22">
         <v>353.51</v>
       </c>
       <c r="F164" s="2">
@@ -11696,7 +11654,7 @@
       <c r="J164" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K164" s="26">
+      <c r="K164" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11710,10 +11668,10 @@
       <c r="C165" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D165" s="25">
+      <c r="D165" s="22">
         <v>593.27</v>
       </c>
-      <c r="E165" s="25">
+      <c r="E165" s="22">
         <v>353.51</v>
       </c>
       <c r="F165" s="2">
@@ -11731,7 +11689,7 @@
       <c r="J165" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K165" s="26">
+      <c r="K165" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11745,10 +11703,10 @@
       <c r="C166" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D166" s="25">
+      <c r="D166" s="22">
         <v>593.27</v>
       </c>
-      <c r="E166" s="25">
+      <c r="E166" s="22">
         <v>353.51</v>
       </c>
       <c r="F166" s="2">
@@ -11766,7 +11724,7 @@
       <c r="J166" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K166" s="26">
+      <c r="K166" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11780,10 +11738,10 @@
       <c r="C167" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D167" s="25">
+      <c r="D167" s="22">
         <v>593.27</v>
       </c>
-      <c r="E167" s="25">
+      <c r="E167" s="22">
         <v>353.51</v>
       </c>
       <c r="F167" s="2">
@@ -11801,7 +11759,7 @@
       <c r="J167" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K167" s="26">
+      <c r="K167" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -11815,10 +11773,10 @@
       <c r="C168" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D168" s="25">
+      <c r="D168" s="22">
         <v>593.27</v>
       </c>
-      <c r="E168" s="25">
+      <c r="E168" s="22">
         <v>353.51</v>
       </c>
       <c r="F168" s="2">
@@ -11836,7 +11794,7 @@
       <c r="J168" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="K168" s="26">
+      <c r="K168" s="23">
         <v>11217</v>
       </c>
     </row>
@@ -11850,10 +11808,10 @@
       <c r="C169" s="2" t="s">
         <v>429</v>
       </c>
-      <c r="D169" s="25">
+      <c r="D169" s="22">
         <v>1949</v>
       </c>
-      <c r="E169" s="25">
+      <c r="E169" s="22">
         <v>1233.1099999999999</v>
       </c>
       <c r="F169" s="2">
@@ -11871,7 +11829,7 @@
       <c r="J169" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="K169" s="26">
+      <c r="K169" s="23">
         <v>12441</v>
       </c>
     </row>
@@ -11885,10 +11843,10 @@
       <c r="C170" s="2" t="s">
         <v>430</v>
       </c>
-      <c r="D170" s="25">
+      <c r="D170" s="22">
         <v>301.24</v>
       </c>
-      <c r="E170" s="25">
+      <c r="E170" s="22">
         <v>116.33</v>
       </c>
       <c r="F170" s="2">
@@ -11906,7 +11864,7 @@
       <c r="J170" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K170" s="26">
+      <c r="K170" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -11920,10 +11878,10 @@
       <c r="C171" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D171" s="25">
+      <c r="D171" s="22">
         <v>2047.5</v>
       </c>
-      <c r="E171" s="25">
+      <c r="E171" s="22">
         <v>1448.85</v>
       </c>
       <c r="F171" s="2">
@@ -11941,7 +11899,7 @@
       <c r="J171" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K171" s="26">
+      <c r="K171" s="23">
         <v>26893</v>
       </c>
     </row>
@@ -11955,10 +11913,10 @@
       <c r="C172" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D172" s="25">
+      <c r="D172" s="22">
         <v>2047.5</v>
       </c>
-      <c r="E172" s="25">
+      <c r="E172" s="22">
         <v>1448.85</v>
       </c>
       <c r="F172" s="2">
@@ -11976,7 +11934,7 @@
       <c r="J172" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="K172" s="26">
+      <c r="K172" s="23">
         <v>26893</v>
       </c>
     </row>
@@ -11990,10 +11948,10 @@
       <c r="C173" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D173" s="25">
+      <c r="D173" s="22">
         <v>838.2</v>
       </c>
-      <c r="E173" s="25">
+      <c r="E173" s="22">
         <v>649.79999999999995</v>
       </c>
       <c r="F173" s="2">
@@ -12011,7 +11969,7 @@
       <c r="J173" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K173" s="26">
+      <c r="K173" s="23">
         <v>506</v>
       </c>
     </row>
@@ -12025,10 +11983,10 @@
       <c r="C174" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="D174" s="25">
+      <c r="D174" s="22">
         <v>838.2</v>
       </c>
-      <c r="E174" s="25">
+      <c r="E174" s="22">
         <v>649.79999999999995</v>
       </c>
       <c r="F174" s="2">
@@ -12046,7 +12004,7 @@
       <c r="J174" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K174" s="26">
+      <c r="K174" s="23">
         <v>506</v>
       </c>
     </row>
@@ -12060,10 +12018,10 @@
       <c r="C175" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="D175" s="25">
+      <c r="D175" s="22">
         <v>329</v>
       </c>
-      <c r="E175" s="25">
+      <c r="E175" s="22">
         <v>262.58</v>
       </c>
       <c r="F175" s="2">
@@ -12081,7 +12039,7 @@
       <c r="J175" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K175" s="26">
+      <c r="K175" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12095,10 +12053,10 @@
       <c r="C176" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="D176" s="25">
+      <c r="D176" s="22">
         <v>3245</v>
       </c>
-      <c r="E176" s="25">
+      <c r="E176" s="22">
         <v>2588.09</v>
       </c>
       <c r="F176" s="2">
@@ -12116,7 +12074,7 @@
       <c r="J176" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K176" s="26">
+      <c r="K176" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12130,10 +12088,10 @@
       <c r="C177" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D177" s="25">
+      <c r="D177" s="22">
         <v>2404</v>
       </c>
-      <c r="E177" s="25">
+      <c r="E177" s="22">
         <v>1917.19</v>
       </c>
       <c r="F177" s="2">
@@ -12151,7 +12109,7 @@
       <c r="J177" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K177" s="26">
+      <c r="K177" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -12165,10 +12123,10 @@
       <c r="C178" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D178" s="25">
+      <c r="D178" s="22">
         <v>2404</v>
       </c>
-      <c r="E178" s="25">
+      <c r="E178" s="22">
         <v>1917.19</v>
       </c>
       <c r="F178" s="2">
@@ -12186,7 +12144,7 @@
       <c r="J178" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K178" s="26">
+      <c r="K178" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -12200,10 +12158,10 @@
       <c r="C179" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D179" s="25">
+      <c r="D179" s="22">
         <v>2404</v>
       </c>
-      <c r="E179" s="25">
+      <c r="E179" s="22">
         <v>1917.19</v>
       </c>
       <c r="F179" s="2">
@@ -12221,7 +12179,7 @@
       <c r="J179" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="K179" s="26">
+      <c r="K179" s="23">
         <v>9510</v>
       </c>
     </row>
@@ -12235,10 +12193,10 @@
       <c r="C180" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D180" s="25">
+      <c r="D180" s="22">
         <v>2404</v>
       </c>
-      <c r="E180" s="25">
+      <c r="E180" s="22">
         <v>1917.19</v>
       </c>
       <c r="F180" s="2">
@@ -12256,7 +12214,7 @@
       <c r="J180" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K180" s="26">
+      <c r="K180" s="23">
         <v>953</v>
       </c>
     </row>
@@ -12270,10 +12228,10 @@
       <c r="C181" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D181" s="25">
+      <c r="D181" s="22">
         <v>2404</v>
       </c>
-      <c r="E181" s="25">
+      <c r="E181" s="22">
         <v>1917.19</v>
       </c>
       <c r="F181" s="2">
@@ -12291,7 +12249,7 @@
       <c r="J181" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="K181" s="26">
+      <c r="K181" s="23">
         <v>9509</v>
       </c>
     </row>
@@ -12305,10 +12263,10 @@
       <c r="C182" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="D182" s="25">
+      <c r="D182" s="22">
         <v>2404</v>
       </c>
-      <c r="E182" s="25">
+      <c r="E182" s="22">
         <v>1917.19</v>
       </c>
       <c r="F182" s="2">
@@ -12326,7 +12284,7 @@
       <c r="J182" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="K182" s="26">
+      <c r="K182" s="23">
         <v>9509</v>
       </c>
     </row>
@@ -12340,10 +12298,10 @@
       <c r="C183" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D183" s="25">
+      <c r="D183" s="22">
         <v>1710</v>
       </c>
-      <c r="E183" s="25">
+      <c r="E183" s="22">
         <v>1222.6500000000001</v>
       </c>
       <c r="F183" s="2">
@@ -12361,7 +12319,7 @@
       <c r="J183" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K183" s="26">
+      <c r="K183" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12375,10 +12333,10 @@
       <c r="C184" s="2" t="s">
         <v>435</v>
       </c>
-      <c r="D184" s="25">
+      <c r="D184" s="22">
         <v>1710</v>
       </c>
-      <c r="E184" s="25">
+      <c r="E184" s="22">
         <v>1222.6500000000001</v>
       </c>
       <c r="F184" s="2">
@@ -12396,7 +12354,7 @@
       <c r="J184" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K184" s="26">
+      <c r="K184" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12410,10 +12368,10 @@
       <c r="C185" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="D185" s="25">
+      <c r="D185" s="22">
         <v>3275</v>
       </c>
-      <c r="E185" s="25">
+      <c r="E185" s="22">
         <v>2341.7199999999998</v>
       </c>
       <c r="F185" s="2">
@@ -12431,7 +12389,7 @@
       <c r="J185" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K185" s="26">
+      <c r="K185" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12445,10 +12403,10 @@
       <c r="C186" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="D186" s="25">
+      <c r="D186" s="22">
         <v>1000</v>
       </c>
-      <c r="E186" s="25">
+      <c r="E186" s="22">
         <v>873.46</v>
       </c>
       <c r="F186" s="2">
@@ -12466,7 +12424,7 @@
       <c r="J186" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="K186" s="26">
+      <c r="K186" s="23">
         <v>12261</v>
       </c>
     </row>
@@ -12480,10 +12438,10 @@
       <c r="C187" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D187" s="25">
+      <c r="D187" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E187" s="25">
+      <c r="E187" s="22">
         <v>975.22</v>
       </c>
       <c r="F187" s="2">
@@ -12501,7 +12459,7 @@
       <c r="J187" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K187" s="26">
+      <c r="K187" s="23">
         <v>953</v>
       </c>
     </row>
@@ -12515,10 +12473,10 @@
       <c r="C188" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D188" s="25">
+      <c r="D188" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E188" s="25">
+      <c r="E188" s="22">
         <v>975.22</v>
       </c>
       <c r="F188" s="2">
@@ -12536,7 +12494,7 @@
       <c r="J188" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K188" s="26">
+      <c r="K188" s="23">
         <v>27049</v>
       </c>
     </row>
@@ -12550,10 +12508,10 @@
       <c r="C189" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D189" s="25">
+      <c r="D189" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E189" s="25">
+      <c r="E189" s="22">
         <v>975.22</v>
       </c>
       <c r="F189" s="2">
@@ -12571,7 +12529,7 @@
       <c r="J189" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K189" s="26">
+      <c r="K189" s="23">
         <v>10517</v>
       </c>
     </row>
@@ -12585,10 +12543,10 @@
       <c r="C190" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D190" s="25">
+      <c r="D190" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E190" s="25">
+      <c r="E190" s="22">
         <v>975.22</v>
       </c>
       <c r="F190" s="2">
@@ -12606,7 +12564,7 @@
       <c r="J190" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="K190" s="26">
+      <c r="K190" s="23">
         <v>27049</v>
       </c>
     </row>
@@ -12620,10 +12578,10 @@
       <c r="C191" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D191" s="25">
+      <c r="D191" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E191" s="25">
+      <c r="E191" s="22">
         <v>975.22</v>
       </c>
       <c r="F191" s="2">
@@ -12641,7 +12599,7 @@
       <c r="J191" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K191" s="26">
+      <c r="K191" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -12655,10 +12613,10 @@
       <c r="C192" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D192" s="25">
+      <c r="D192" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E192" s="25">
+      <c r="E192" s="22">
         <v>975.22</v>
       </c>
       <c r="F192" s="2">
@@ -12676,7 +12634,7 @@
       <c r="J192" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="K192" s="26">
+      <c r="K192" s="23">
         <v>26413</v>
       </c>
     </row>
@@ -12690,10 +12648,10 @@
       <c r="C193" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="D193" s="25">
+      <c r="D193" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E193" s="25">
+      <c r="E193" s="22">
         <v>975.22</v>
       </c>
       <c r="F193" s="2">
@@ -12711,7 +12669,7 @@
       <c r="J193" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="K193" s="26">
+      <c r="K193" s="23">
         <v>26414</v>
       </c>
     </row>
@@ -12725,10 +12683,10 @@
       <c r="C194" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D194" s="25">
+      <c r="D194" s="22">
         <v>1200</v>
       </c>
-      <c r="E194" s="25">
+      <c r="E194" s="22">
         <v>1092</v>
       </c>
       <c r="F194" s="2">
@@ -12746,7 +12704,7 @@
       <c r="J194" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K194" s="26">
+      <c r="K194" s="23">
         <v>9701</v>
       </c>
     </row>
@@ -12760,10 +12718,10 @@
       <c r="C195" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D195" s="25">
+      <c r="D195" s="22">
         <v>1200</v>
       </c>
-      <c r="E195" s="25">
+      <c r="E195" s="22">
         <v>1092</v>
       </c>
       <c r="F195" s="2">
@@ -12781,7 +12739,7 @@
       <c r="J195" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K195" s="26">
+      <c r="K195" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -12795,10 +12753,10 @@
       <c r="C196" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="D196" s="25">
+      <c r="D196" s="22">
         <v>1200</v>
       </c>
-      <c r="E196" s="25">
+      <c r="E196" s="22">
         <v>1092</v>
       </c>
       <c r="F196" s="2">
@@ -12816,7 +12774,7 @@
       <c r="J196" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="K196" s="26">
+      <c r="K196" s="23">
         <v>9613</v>
       </c>
     </row>
@@ -12841,54 +12799,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>441</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>443</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>444</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>447</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>449</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>450</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>454</v>
       </c>
     </row>
@@ -12899,19 +12858,19 @@
       <c r="B2" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45108</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="28">
         <v>4812</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="28" t="s">
         <v>456</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>50744</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>3570</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -12920,22 +12879,22 @@
       <c r="I2" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>458</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>459</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>459</v>
       </c>
     </row>
@@ -12966,25 +12925,24 @@
       <c r="B1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>461</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>292</v>
+      </c>
+      <c r="B2" s="36">
         <v>153</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>292</v>
-      </c>
-      <c r="B2" s="39">
-        <v>153</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>1.0117709297711939E-2</v>
       </c>
     </row>

</xml_diff>